<commit_message>
Overall evaluation report for the application
</commit_message>
<xml_diff>
--- a/Test-docs/Mobile QA assignment report.xlsx
+++ b/Test-docs/Mobile QA assignment report.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="80" windowWidth="19140" windowHeight="7340" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="80" windowWidth="19140" windowHeight="7340"/>
   </bookViews>
   <sheets>
     <sheet name="Manual Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="Evaluation report" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="94">
   <si>
     <t>Test case #</t>
   </si>
@@ -468,9 +467,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -486,6 +482,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -791,7 +790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -807,10 +806,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="15"/>
+      <c r="B1" s="14"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
@@ -881,7 +880,7 @@
       <c r="A5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>66</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -902,7 +901,7 @@
       <c r="A6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>62</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -923,7 +922,7 @@
       <c r="A7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>34</v>
       </c>
       <c r="C7" s="6" t="s">
@@ -944,7 +943,7 @@
       <c r="A8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>59</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -965,7 +964,7 @@
       <c r="A9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>58</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -986,7 +985,7 @@
       <c r="A10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>55</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -1100,8 +1099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1113,10 +1112,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="31" x14ac:dyDescent="0.7">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="9"/>
+      <c r="B1" s="15"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -1206,58 +1205,67 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="B16" s="11"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B16" s="10"/>
+      <c r="C16" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B17" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="11" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B19" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>80</v>
       </c>
       <c r="B20" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="11" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="87" x14ac:dyDescent="0.35">
-      <c r="A22" s="13" t="s">
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+      <c r="A22" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="13" t="s">
         <v>90</v>
       </c>
+      <c r="C22" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>